<commit_message>
Optimization BC Workspace and Transformers
</commit_message>
<xml_diff>
--- a/FME_fmw_files/LOOKUP_TABLES/RoleAttributeMapper.xlsx
+++ b/FME_fmw_files/LOOKUP_TABLES/RoleAttributeMapper.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>original_value</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>resourceProvider</t>
+  </si>
+  <si>
+    <t>businessExpert</t>
   </si>
 </sst>
 </file>
@@ -488,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,6 +729,20 @@
         <v>4</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>